<commit_message>
Update template data files
Now these include more comprehensive examples

https://github.com/MTG/freesound/pull/1093
</commit_message>
<xml_diff>
--- a/media/sample.xlsx
+++ b/media/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10522"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ffont/Developer/Freesound/freesound/media/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF6D238F-334F-C54B-809C-D09747537837}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE3D99D-42BE-054C-9724-2C525E67378C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{74EB3FE5-2690-344D-9F4D-E29FA9C96C71}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>audio_filename</t>
   </si>
@@ -54,41 +54,62 @@
     <t>Creative Commons 0</t>
   </si>
   <si>
-    <t>filename.wav</t>
-  </si>
-  <si>
-    <t>A cool name for my sound</t>
-  </si>
-  <si>
-    <t>tag1 tag2 tag3 separated-by-spaces</t>
-  </si>
-  <si>
-    <t>lat, lng, zoom</t>
-  </si>
-  <si>
-    <t>The textual description for the sound.</t>
-  </si>
-  <si>
-    <t>My pack</t>
+    <t>heart beat.mp3</t>
+  </si>
+  <si>
+    <t>low-frequency beat heart heartbeat</t>
+  </si>
+  <si>
+    <t>This was produced by tapping on a stethoscope which had an earbud pressed against a Shure SM57 mic. Low pass filter applied, as well as compression and a gate. Chorus added. Used a recording cassette deck as a preamp going into an M-Audio Audiophile USB soundcard.
+Note: If you're having problems listening to this clip, the cutoff frequency of your speaker set may be too high(solution: new speakers). The signal strength exists almost entirely in the very low frequencies, so you may need a sub-woofer to hear it. Otherwise, try turning your speaker volume all the way up. Doing so may saturate the signal and at least allow you to hear the harmonics of the signal caused by the distortion. I don't recommend it, but you'll at least maybe be able to hear something.</t>
+  </si>
+  <si>
+    <t>rbh thunder storm.wav</t>
+  </si>
+  <si>
+    <t>siren xy stereo heavy-rain thunder-storm storm nature field-recording rain thunder purist weather lightning</t>
+  </si>
+  <si>
+    <t>rain and several thunder claps. Stereo. Recorded with a minidisc recorder and an AT822 mic. Edited in Protools and saved as a 48/16 wav file.
+I have more sounds available here:
+http://sfx.TakomaMedia.com</t>
+  </si>
+  <si>
+    <t>Attribution</t>
+  </si>
+  <si>
+    <t>Storm</t>
+  </si>
+  <si>
+    <t>STEREO_41.wav</t>
+  </si>
+  <si>
+    <t>Close seashore - Saintes-Maries-de-la-Mer</t>
+  </si>
+  <si>
+    <t>shure-mv88 beach close waves sea seashore shore water field-recording</t>
+  </si>
+  <si>
+    <t>43.44902, 4.40802, 16</t>
+  </si>
+  <si>
+    <t>Close recording of the seashore in Saintes-Maries-de-la-Mer, Provence-Alpes-Côte d'Azur, France. Recorded with my mobile phone with a Shure mv88 on August 2015.</t>
+  </si>
+  <si>
+    <t>Provence-Alpes-Côte d'Azur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,7 +134,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,9 +451,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{232366E6-B125-BD44-A55D-75C8966C8991}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -438,7 +463,7 @@
     <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.1640625" customWidth="1"/>
     <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -470,33 +495,79 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="G2" s="1"/>
       <c r="H2" s="1">
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="96" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" display="https://freesound.org/people/frederic.font/sounds/322271/" xr:uid="{CB60B5F3-B9A1-BB4B-BD6F-BD26A9060706}"/>
+    <hyperlink ref="A2" r:id="rId2" display="https://freesound.org/people/greyseraphim/sounds/21409/" xr:uid="{AF094151-9857-3F4E-95B1-25C5A892086C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Add "Attribution Noncommerical" example in sample data files
https://github.com/MTG/freesound/pull/1093
</commit_message>
<xml_diff>
--- a/media/sample.xlsx
+++ b/media/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10522"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ffont/Developer/Freesound/freesound/media/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE3D99D-42BE-054C-9724-2C525E67378C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600330B8-5C4E-D24F-AE2A-910B93E2F2C1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{74EB3FE5-2690-344D-9F4D-E29FA9C96C71}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>audio_filename</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Provence-Alpes-Côte d'Azur</t>
+  </si>
+  <si>
+    <t>Attribution Noncommercial</t>
   </si>
 </sst>
 </file>
@@ -454,7 +457,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,7 +557,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>22</v>

</xml_diff>